<commit_message>
Added iam-vulnerable, sadcloud, and terragoat as submodules
</commit_message>
<xml_diff>
--- a/docs/Checkov risk categories.xlsx
+++ b/docs/Checkov risk categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmcquade/Code/github.com/kmcquade/terraform-aws-vulnerable/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C617D112-3317-CC41-827C-21A6CC290426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB192760-21C6-9B48-A202-B9FAF7743285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9D04EDE8-B811-AF46-BE8F-A8BDD363BB19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="580">
   <si>
     <t>Id</t>
   </si>
@@ -1671,9 +1671,6 @@
     <t>Network Exposure</t>
   </si>
   <si>
-    <t>Allowed Usage</t>
-  </si>
-  <si>
     <t>Multiple</t>
   </si>
   <si>
@@ -1795,6 +1792,9 @@
   </si>
   <si>
     <t>Log retention</t>
+  </si>
+  <si>
+    <t>VPC Flow logs</t>
   </si>
 </sst>
 </file>
@@ -2387,17 +2387,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951614AF-2C4D-E143-9FB7-50433CD8548C}">
   <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="E227" sqref="E227"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
     <col min="7" max="7" width="56.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="97.5" customWidth="1"/>
   </cols>
@@ -2583,7 +2583,7 @@
         <v>507</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>23</v>
@@ -2896,7 +2896,7 @@
         <v>519</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>45</v>
@@ -2925,7 +2925,7 @@
         <v>519</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>49</v>
@@ -3010,7 +3010,7 @@
         <v>519</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>51</v>
@@ -3036,7 +3036,7 @@
         <v>524</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>522</v>
@@ -3094,7 +3094,7 @@
         <v>511</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>521</v>
@@ -3123,7 +3123,7 @@
         <v>511</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>521</v>
@@ -3152,7 +3152,7 @@
         <v>511</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>521</v>
@@ -3181,7 +3181,7 @@
         <v>511</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>521</v>
@@ -3210,7 +3210,7 @@
         <v>526</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>521</v>
@@ -3512,7 +3512,7 @@
         <v>519</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>90</v>
@@ -3541,7 +3541,7 @@
         <v>519</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>23</v>
@@ -3567,7 +3567,7 @@
         <v>533</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
@@ -3626,7 +3626,7 @@
         <v>520</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>98</v>
@@ -3735,7 +3735,7 @@
         <v>509</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>538</v>
+        <v>568</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>521</v>
@@ -3764,7 +3764,7 @@
         <v>509</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>521</v>
@@ -3793,7 +3793,7 @@
         <v>509</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>538</v>
+        <v>568</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>521</v>
@@ -3819,10 +3819,10 @@
         <v>115</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2" t="s">
@@ -3846,7 +3846,7 @@
         <v>11</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>507</v>
@@ -3875,7 +3875,7 @@
         <v>11</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>507</v>
@@ -3904,7 +3904,7 @@
         <v>11</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>507</v>
@@ -3933,10 +3933,10 @@
         <v>11</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2" t="s">
@@ -3963,7 +3963,7 @@
         <v>511</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2" t="s">
@@ -4016,7 +4016,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>520</v>
@@ -4072,7 +4072,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>520</v>
@@ -4104,10 +4104,10 @@
         <v>532</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>143</v>
@@ -4136,7 +4136,7 @@
         <v>519</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>146</v>
@@ -4165,7 +4165,7 @@
         <v>519</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>146</v>
@@ -4194,7 +4194,7 @@
         <v>519</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>146</v>
@@ -4223,7 +4223,7 @@
         <v>519</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>146</v>
@@ -4252,7 +4252,7 @@
         <v>519</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>51</v>
@@ -4304,13 +4304,13 @@
         <v>11</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>519</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>159</v>
@@ -4339,7 +4339,7 @@
         <v>519</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>162</v>
@@ -4368,7 +4368,7 @@
         <v>519</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>162</v>
@@ -4499,7 +4499,7 @@
         <v>11</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>508</v>
@@ -4634,7 +4634,7 @@
         <v>11</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>508</v>
@@ -4690,7 +4690,7 @@
         <v>11</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>520</v>
@@ -4719,13 +4719,13 @@
         <v>11</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>520</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>179</v>
@@ -4754,7 +4754,7 @@
         <v>520</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>98</v>
@@ -4780,10 +4780,10 @@
         <v>533</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>95</v>
@@ -4806,7 +4806,7 @@
         <v>11</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>537</v>
@@ -4893,7 +4893,7 @@
         <v>520</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>173</v>
@@ -4943,7 +4943,7 @@
         <v>11</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>520</v>
@@ -4972,7 +4972,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>507</v>
@@ -5001,13 +5001,13 @@
         <v>11</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>520</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>202</v>
@@ -5030,13 +5030,13 @@
         <v>11</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>520</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>196</v>
@@ -5059,13 +5059,13 @@
         <v>11</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>520</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>206</v>
@@ -5088,7 +5088,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>507</v>
@@ -5117,7 +5117,7 @@
         <v>11</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>507</v>
@@ -5149,7 +5149,7 @@
         <v>511</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2" t="s">
@@ -5176,7 +5176,7 @@
         <v>511</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2" t="s">
@@ -5200,13 +5200,13 @@
         <v>11</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>520</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>217</v>
@@ -5229,7 +5229,7 @@
         <v>11</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>506</v>
@@ -5256,7 +5256,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>507</v>
@@ -5283,7 +5283,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>507</v>
@@ -5345,7 +5345,7 @@
         <v>520</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>18</v>
@@ -5368,7 +5368,7 @@
         <v>11</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>520</v>
@@ -5403,7 +5403,7 @@
         <v>520</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>95</v>
@@ -5507,7 +5507,7 @@
         <v>11</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>537</v>
@@ -5534,7 +5534,7 @@
         <v>11</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>506</v>
@@ -5567,7 +5567,7 @@
         <v>520</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>243</v>
@@ -5596,7 +5596,7 @@
         <v>520</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>245</v>
@@ -5625,7 +5625,7 @@
         <v>520</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>247</v>
@@ -5651,10 +5651,10 @@
         <v>524</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>51</v>
@@ -5680,10 +5680,10 @@
         <v>524</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>189</v>
@@ -5812,7 +5812,7 @@
         <v>11</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>507</v>
@@ -5868,13 +5868,13 @@
         <v>11</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>520</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>125</v>
@@ -5951,7 +5951,7 @@
         <v>520</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>240</v>
@@ -6032,7 +6032,7 @@
         <v>508</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G130" s="2" t="s">
         <v>7</v>
@@ -6061,7 +6061,7 @@
         <v>508</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>7</v>
@@ -6090,7 +6090,7 @@
         <v>508</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>7</v>
@@ -6119,7 +6119,7 @@
         <v>508</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>7</v>
@@ -6148,7 +6148,7 @@
         <v>508</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>7</v>
@@ -6245,10 +6245,10 @@
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>128</v>
@@ -6272,10 +6272,10 @@
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>128</v>
@@ -6403,10 +6403,10 @@
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>196</v>
@@ -6433,7 +6433,7 @@
         <v>520</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>315</v>
@@ -6482,10 +6482,10 @@
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>320</v>
@@ -6509,10 +6509,10 @@
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>323</v>
@@ -6588,10 +6588,10 @@
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F151" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>255</v>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F154" s="2"/>
       <c r="G154" s="2" t="s">
@@ -6692,7 +6692,7 @@
       </c>
       <c r="D155" s="2"/>
       <c r="E155" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F155" s="2"/>
       <c r="G155" s="2" t="s">
@@ -6715,7 +6715,9 @@
       <c r="C156" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D156" s="2"/>
+      <c r="D156" s="2" t="s">
+        <v>518</v>
+      </c>
       <c r="E156" s="2" t="s">
         <v>529</v>
       </c>
@@ -6740,7 +6742,9 @@
       <c r="C157" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D157" s="2"/>
+      <c r="D157" s="2" t="s">
+        <v>531</v>
+      </c>
       <c r="E157" s="2" t="s">
         <v>529</v>
       </c>
@@ -6767,10 +6771,10 @@
       </c>
       <c r="D158" s="2"/>
       <c r="E158" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F158" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G158" s="2" t="s">
         <v>26</v>
@@ -6846,10 +6850,10 @@
       </c>
       <c r="D161" s="2"/>
       <c r="E161" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G161" s="2" t="s">
         <v>247</v>
@@ -6873,7 +6877,7 @@
       </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>522</v>
@@ -6927,10 +6931,10 @@
       </c>
       <c r="D164" s="2"/>
       <c r="E164" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F164" s="2" t="s">
         <v>575</v>
-      </c>
-      <c r="F164" s="2" t="s">
-        <v>576</v>
       </c>
       <c r="G164" s="2" t="s">
         <v>173</v>
@@ -6981,10 +6985,10 @@
       </c>
       <c r="D166" s="2"/>
       <c r="E166" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F166" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F166" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>51</v>
@@ -7008,10 +7012,10 @@
       </c>
       <c r="D167" s="2"/>
       <c r="E167" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F167" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F167" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G167" s="2" t="s">
         <v>51</v>
@@ -7119,7 +7123,7 @@
         <v>537</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G171" s="2" t="s">
         <v>372</v>
@@ -7170,7 +7174,7 @@
       </c>
       <c r="D173" s="2"/>
       <c r="E173" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>522</v>
@@ -7197,7 +7201,7 @@
       </c>
       <c r="D174" s="2"/>
       <c r="E174" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>522</v>
@@ -7224,10 +7228,10 @@
       </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G175" s="2" t="s">
         <v>243</v>
@@ -7251,10 +7255,10 @@
       </c>
       <c r="D176" s="2"/>
       <c r="E176" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G176" s="2" t="s">
         <v>245</v>
@@ -7278,7 +7282,7 @@
       </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F177" s="2"/>
       <c r="G177" s="2" t="s">
@@ -7378,7 +7382,7 @@
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>522</v>
@@ -7486,10 +7490,10 @@
       </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F185" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F185" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G185" s="2" t="s">
         <v>45</v>
@@ -7513,10 +7517,10 @@
       </c>
       <c r="D186" s="2"/>
       <c r="E186" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F186" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F186" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G186" s="2" t="s">
         <v>255</v>
@@ -7540,10 +7544,10 @@
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F187" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="F187" s="2" t="s">
-        <v>570</v>
       </c>
       <c r="G187" s="2" t="s">
         <v>143</v>
@@ -7592,10 +7596,10 @@
       </c>
       <c r="D189" s="2"/>
       <c r="E189" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G189" s="2" t="s">
         <v>410</v>
@@ -7769,10 +7773,10 @@
       </c>
       <c r="D196" s="2"/>
       <c r="E196" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G196" s="2" t="s">
         <v>424</v>
@@ -7821,10 +7825,10 @@
       </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G198" s="2" t="s">
         <v>434</v>
@@ -7848,10 +7852,10 @@
       </c>
       <c r="D199" s="2"/>
       <c r="E199" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G199" s="2" t="s">
         <v>334</v>
@@ -7928,7 +7932,7 @@
         <v>520</v>
       </c>
       <c r="F202" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G202" s="2" t="s">
         <v>440</v>
@@ -7955,7 +7959,7 @@
         <v>520</v>
       </c>
       <c r="F203" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G203" s="2" t="s">
         <v>442</v>
@@ -8033,10 +8037,10 @@
       </c>
       <c r="D206" s="2"/>
       <c r="E206" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F206" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G206" s="2" t="s">
         <v>63</v>
@@ -8158,7 +8162,9 @@
       <c r="C211" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D211" s="2"/>
+      <c r="D211" s="2" t="s">
+        <v>518</v>
+      </c>
       <c r="E211" s="2" t="s">
         <v>529</v>
       </c>
@@ -8183,7 +8189,9 @@
       <c r="C212" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D212" s="2"/>
+      <c r="D212" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="E212" s="2" t="s">
         <v>529</v>
       </c>
@@ -8215,7 +8223,7 @@
         <v>520</v>
       </c>
       <c r="F213" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G213" s="2" t="s">
         <v>98</v>
@@ -8242,7 +8250,7 @@
         <v>520</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>556</v>
+        <v>579</v>
       </c>
       <c r="G214" s="2" t="s">
         <v>460</v>
@@ -8266,10 +8274,10 @@
       </c>
       <c r="D215" s="2"/>
       <c r="E215" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G215" s="2" t="s">
         <v>460</v>
@@ -8293,10 +8301,10 @@
       </c>
       <c r="D216" s="2"/>
       <c r="E216" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F216" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G216" s="2" t="s">
         <v>464</v>
@@ -8318,7 +8326,9 @@
       <c r="C217" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D217" s="2"/>
+      <c r="D217" s="2" t="s">
+        <v>526</v>
+      </c>
       <c r="E217" s="2" t="s">
         <v>529</v>
       </c>
@@ -8345,10 +8355,10 @@
       </c>
       <c r="D218" s="2"/>
       <c r="E218" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F218" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G218" s="2" t="s">
         <v>468</v>
@@ -8372,10 +8382,10 @@
       </c>
       <c r="D219" s="2"/>
       <c r="E219" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F219" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G219" s="2" t="s">
         <v>470</v>
@@ -8399,10 +8409,10 @@
       </c>
       <c r="D220" s="2"/>
       <c r="E220" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F220" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G220" s="2" t="s">
         <v>382</v>
@@ -8426,10 +8436,10 @@
       </c>
       <c r="D221" s="2"/>
       <c r="E221" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G221" s="2" t="s">
         <v>247</v>
@@ -8453,10 +8463,10 @@
       </c>
       <c r="D222" s="2"/>
       <c r="E222" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F222" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G222" s="2" t="s">
         <v>80</v>
@@ -8480,10 +8490,10 @@
       </c>
       <c r="D223" s="2"/>
       <c r="E223" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F223" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G223" s="2" t="s">
         <v>475</v>
@@ -8505,7 +8515,9 @@
       <c r="C224" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D224" s="2"/>
+      <c r="D224" s="2" t="s">
+        <v>540</v>
+      </c>
       <c r="E224" s="2" t="s">
         <v>529</v>
       </c>
@@ -8532,10 +8544,10 @@
       </c>
       <c r="D225" s="2"/>
       <c r="E225" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F225" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G225" s="2" t="s">
         <v>479</v>
@@ -8559,10 +8571,10 @@
       </c>
       <c r="D226" s="2"/>
       <c r="E226" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F226" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G226" s="2" t="s">
         <v>481</v>
@@ -8638,10 +8650,10 @@
         <v>509</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F229" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G229" s="2" t="s">
         <v>470</v>
@@ -8667,10 +8679,10 @@
         <v>509</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F230" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G230" s="2" t="s">
         <v>487</v>
@@ -8697,7 +8709,7 @@
         <v>519</v>
       </c>
       <c r="F231" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G231" s="2" t="s">
         <v>490</v>
@@ -8775,10 +8787,10 @@
       </c>
       <c r="D234" s="2"/>
       <c r="E234" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F234" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G234" s="2" t="s">
         <v>243</v>
@@ -8802,10 +8814,10 @@
       </c>
       <c r="D235" s="2"/>
       <c r="E235" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F235" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G235" s="2" t="s">
         <v>498</v>
@@ -8829,10 +8841,10 @@
       </c>
       <c r="D236" s="2"/>
       <c r="E236" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F236" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G236" s="2" t="s">
         <v>196</v>
@@ -8900,6 +8912,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>